<commit_message>
ANCOVA with all covariates
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/10_KCAL means.xlsx
+++ b/eg_data/NHANES/PF/10_KCAL means.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DC8558-A528-4BFE-A5D6-8C4BABAFFCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB7F726-C7ED-4AE6-849A-348AD4A489BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31605" yWindow="-3105" windowWidth="17175" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32775" yWindow="-3270" windowWidth="15615" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KCAL" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="77">
   <si>
     <t>Plain means</t>
   </si>
@@ -214,6 +214,60 @@
   </si>
   <si>
     <t>FIBE n</t>
+  </si>
+  <si>
+    <t>DivGroup, Age, Gender, FIBE, PF</t>
+  </si>
+  <si>
+    <t>lm.kcal.agfp &lt;-    lm( BMXWAIST ~ DivGroup + RIDAGEYR + Gender + FIBE + PF_TOTAL_LEG, data=df)</t>
+  </si>
+  <si>
+    <t>Sum Sq</t>
+  </si>
+  <si>
+    <t>Df</t>
+  </si>
+  <si>
+    <t>F value</t>
+  </si>
+  <si>
+    <t>Pr(&gt;F)</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>RIDAGEYR</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Residuals</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>All terms have an effect.</t>
+  </si>
+  <si>
+    <t>The more diverse, the less KCAL intake.</t>
+  </si>
+  <si>
+    <t>DivGroup, Age, Gender, FIBE/1000kcal, PF</t>
+  </si>
+  <si>
+    <t>FIBE1000kcal</t>
+  </si>
+  <si>
+    <t>lm.kcal.ag1000fp &lt;-    lm( KCAL ~ DivGroup + RIDAGEYR + Gender + FIBE1000kcal + PF_TOTAL_LEG, data=df)</t>
+  </si>
+  <si>
+    <t>The more diverse, the more kcal intake!</t>
+  </si>
+  <si>
+    <t>When KCAL is the response, I don't quite understand the meaning of adjusting it by FiBE/1000kcal…?</t>
   </si>
 </sst>
 </file>
@@ -224,7 +278,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,8 +331,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +348,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -464,6 +530,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4221,10 +4296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M110" sqref="M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5618,6 +5693,861 @@
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>61</v>
+      </c>
+      <c r="C98" t="s">
+        <v>62</v>
+      </c>
+      <c r="D98" t="s">
+        <v>63</v>
+      </c>
+      <c r="E98" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>65</v>
+      </c>
+      <c r="C99">
+        <v>373179779.51554</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>1398.0876964260401</v>
+      </c>
+      <c r="F99" s="16">
+        <v>5.8851966731691299E-263</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100">
+        <v>51910403.856978402</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+      <c r="E100">
+        <v>64.826035539908204</v>
+      </c>
+      <c r="F100" s="16">
+        <v>6.2428351805183905E-41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>66</v>
+      </c>
+      <c r="C101">
+        <v>30579869.1270709</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>114.564992884605</v>
+      </c>
+      <c r="F101" s="16">
+        <v>2.2097303100334501E-26</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>67</v>
+      </c>
+      <c r="C102">
+        <v>63249633.913745403</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>236.959609904524</v>
+      </c>
+      <c r="F102" s="16">
+        <v>5.3210318097224899E-52</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>34</v>
+      </c>
+      <c r="C103">
+        <v>309367628.46933103</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>1159.0206618294601</v>
+      </c>
+      <c r="F103" s="16">
+        <v>1.64805229437945E-223</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104">
+        <v>222657032.56821701</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>834.16646571922297</v>
+      </c>
+      <c r="F104" s="16">
+        <v>7.0680972260306296E-167</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>68</v>
+      </c>
+      <c r="C105">
+        <v>1075693974.91453</v>
+      </c>
+      <c r="D105">
+        <v>4030</v>
+      </c>
+      <c r="E105" t="s">
+        <v>69</v>
+      </c>
+      <c r="F105" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H107" s="5"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" s="1">
+        <v>2128.4662666589502</v>
+      </c>
+      <c r="D108" s="1">
+        <v>12.130735506751799</v>
+      </c>
+      <c r="E108">
+        <v>4030</v>
+      </c>
+      <c r="F108" s="16">
+        <v>2094.3961162056899</v>
+      </c>
+      <c r="G108">
+        <v>2162.5364171122101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="1">
+        <v>1978.9337204506101</v>
+      </c>
+      <c r="D109" s="1">
+        <v>14.726278107830099</v>
+      </c>
+      <c r="E109">
+        <v>4030</v>
+      </c>
+      <c r="F109" s="16">
+        <v>1937.5737789638699</v>
+      </c>
+      <c r="G109">
+        <v>2020.29366193735</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" t="s">
+        <v>13</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1827.9568880014001</v>
+      </c>
+      <c r="D110" s="1">
+        <v>27.095263567446601</v>
+      </c>
+      <c r="E110">
+        <v>4030</v>
+      </c>
+      <c r="F110" s="16">
+        <v>1751.85765182566</v>
+      </c>
+      <c r="G110">
+        <v>1904.05612417713</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111" s="1">
+        <v>1749.2452311612501</v>
+      </c>
+      <c r="D111" s="1">
+        <v>27.8926427048157</v>
+      </c>
+      <c r="E111">
+        <v>4030</v>
+      </c>
+      <c r="F111" s="16">
+        <v>1670.90649127502</v>
+      </c>
+      <c r="G111">
+        <v>1827.58397104748</v>
+      </c>
+      <c r="H111" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112" s="6">
+        <v>149.53254620834099</v>
+      </c>
+      <c r="D112" s="6">
+        <v>19.3493418863209</v>
+      </c>
+      <c r="E112" s="2">
+        <v>4030</v>
+      </c>
+      <c r="F112" s="17">
+        <v>95.188356701315897</v>
+      </c>
+      <c r="G112" s="2">
+        <v>203.87673571536601</v>
+      </c>
+      <c r="H112" s="17">
+        <v>2.6881694537017599E-8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B113" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" s="56">
+        <v>300.50937865755498</v>
+      </c>
+      <c r="D113" s="56">
+        <v>30.516304364119598</v>
+      </c>
+      <c r="E113" s="51">
+        <v>4030</v>
+      </c>
+      <c r="F113" s="51">
+        <v>214.801873091684</v>
+      </c>
+      <c r="G113" s="51">
+        <v>386.21688422342498</v>
+      </c>
+      <c r="H113" s="52">
+        <v>2.68816225945656E-8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C114" s="57">
+        <v>379.22103549770401</v>
+      </c>
+      <c r="D114" s="56">
+        <v>31.623306395223199</v>
+      </c>
+      <c r="E114" s="51">
+        <v>4030</v>
+      </c>
+      <c r="F114" s="51">
+        <v>290.40442531647301</v>
+      </c>
+      <c r="G114" s="51">
+        <v>468.03764567893501</v>
+      </c>
+      <c r="H114" s="55">
+        <v>2.6881583403692801E-8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B115" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115" s="56">
+        <v>150.97683244921399</v>
+      </c>
+      <c r="D115" s="56">
+        <v>30.527136975646702</v>
+      </c>
+      <c r="E115" s="51">
+        <v>4030</v>
+      </c>
+      <c r="F115" s="51">
+        <v>65.238902618934503</v>
+      </c>
+      <c r="G115" s="51">
+        <v>236.71476227949299</v>
+      </c>
+      <c r="H115" s="52">
+        <v>4.7348925935608602E-6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B116" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C116" s="57">
+        <v>229.68848928936299</v>
+      </c>
+      <c r="D116" s="56">
+        <v>31.106687790891399</v>
+      </c>
+      <c r="E116" s="51">
+        <v>4030</v>
+      </c>
+      <c r="F116" s="51">
+        <v>142.32284418495999</v>
+      </c>
+      <c r="G116" s="51">
+        <v>317.05413439376599</v>
+      </c>
+      <c r="H116" s="55">
+        <v>2.6882725157051401E-8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B117" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117" s="58">
+        <v>78.711656840149303</v>
+      </c>
+      <c r="D117" s="4">
+        <v>37.151417083916598</v>
+      </c>
+      <c r="E117" s="3">
+        <v>4030</v>
+      </c>
+      <c r="F117" s="3">
+        <v>-25.631098708049102</v>
+      </c>
+      <c r="G117" s="3">
+        <v>183.054412388348</v>
+      </c>
+      <c r="H117" s="3">
+        <v>0.14728034949558899</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>61</v>
+      </c>
+      <c r="D124" t="s">
+        <v>62</v>
+      </c>
+      <c r="E124" t="s">
+        <v>63</v>
+      </c>
+      <c r="F124" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>65</v>
+      </c>
+      <c r="C125">
+        <v>709833089.27832401</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <v>2137.99822561173</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126">
+        <v>9162173.4489710294</v>
+      </c>
+      <c r="D126">
+        <v>3</v>
+      </c>
+      <c r="E126">
+        <v>9.1987402261765201</v>
+      </c>
+      <c r="F126" s="16">
+        <v>4.6120846967502999E-6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>66</v>
+      </c>
+      <c r="C127">
+        <v>19112705.601948999</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>57.5669566280026</v>
+      </c>
+      <c r="F127" s="16">
+        <v>4.0327700314543797E-14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>67</v>
+      </c>
+      <c r="C128">
+        <v>97742726.029083699</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128">
+        <v>294.39846912334701</v>
+      </c>
+      <c r="F128" s="16">
+        <v>9.5645833220882601E-64</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>73</v>
+      </c>
+      <c r="C129">
+        <v>47068280.693823799</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>141.76839897433001</v>
+      </c>
+      <c r="F129" s="16">
+        <v>3.7592943636252998E-32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>33</v>
+      </c>
+      <c r="C130">
+        <v>339374647.087915</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>1022.1873342496</v>
+      </c>
+      <c r="F130" s="16">
+        <v>4.2111066516711199E-200</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>68</v>
+      </c>
+      <c r="C131">
+        <v>1337993322.6900401</v>
+      </c>
+      <c r="D131">
+        <v>4030</v>
+      </c>
+      <c r="E131" t="s">
+        <v>69</v>
+      </c>
+      <c r="F131" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>1</v>
+      </c>
+      <c r="B134" t="s">
+        <v>13</v>
+      </c>
+      <c r="C134" s="1">
+        <v>1977.15672849103</v>
+      </c>
+      <c r="D134" s="1">
+        <v>13.6563338055635</v>
+      </c>
+      <c r="E134">
+        <v>4030</v>
+      </c>
+      <c r="F134">
+        <v>1938.80181199512</v>
+      </c>
+      <c r="G134">
+        <v>2015.5116449869499</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" t="s">
+        <v>13</v>
+      </c>
+      <c r="C135" s="1">
+        <v>2020.70670468556</v>
+      </c>
+      <c r="D135" s="1">
+        <v>16.4368928850663</v>
+      </c>
+      <c r="E135">
+        <v>4030</v>
+      </c>
+      <c r="F135">
+        <v>1974.54236343299</v>
+      </c>
+      <c r="G135">
+        <v>2066.87104593813</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136" t="s">
+        <v>13</v>
+      </c>
+      <c r="C136" s="1">
+        <v>2088.00107638999</v>
+      </c>
+      <c r="D136" s="1">
+        <v>30.334330472387201</v>
+      </c>
+      <c r="E136">
+        <v>4030</v>
+      </c>
+      <c r="F136">
+        <v>2002.80465919683</v>
+      </c>
+      <c r="G136">
+        <v>2173.1974935831499</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>4</v>
+      </c>
+      <c r="B137" t="s">
+        <v>13</v>
+      </c>
+      <c r="C137" s="1">
+        <v>2151.7802221952802</v>
+      </c>
+      <c r="D137" s="1">
+        <v>31.174938955120801</v>
+      </c>
+      <c r="E137">
+        <v>4030</v>
+      </c>
+      <c r="F137">
+        <v>2064.2228881835799</v>
+      </c>
+      <c r="G137">
+        <v>2239.33755620697</v>
+      </c>
+      <c r="H137" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C138" s="6">
+        <v>-43.549976194526202</v>
+      </c>
+      <c r="D138" s="6">
+        <v>21.7272074469534</v>
+      </c>
+      <c r="E138" s="2">
+        <v>4030</v>
+      </c>
+      <c r="F138" s="2">
+        <v>-104.572593185465</v>
+      </c>
+      <c r="G138" s="2">
+        <v>17.472640796412499</v>
+      </c>
+      <c r="H138" s="2">
+        <v>0.186446366606354</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B139" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C139" s="56">
+        <v>-110.844347898954</v>
+      </c>
+      <c r="D139" s="56">
+        <v>34.333387241538297</v>
+      </c>
+      <c r="E139" s="51">
+        <v>4030</v>
+      </c>
+      <c r="F139" s="51">
+        <v>-207.27243902650201</v>
+      </c>
+      <c r="G139" s="51">
+        <v>-14.4162567714051</v>
+      </c>
+      <c r="H139" s="51">
+        <v>6.8741851637872404E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B140" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C140" s="57">
+        <v>-174.62349370423999</v>
+      </c>
+      <c r="D140" s="56">
+        <v>35.526052067048802</v>
+      </c>
+      <c r="E140" s="51">
+        <v>4030</v>
+      </c>
+      <c r="F140" s="51">
+        <v>-274.40128032410502</v>
+      </c>
+      <c r="G140" s="51">
+        <v>-74.845707084375107</v>
+      </c>
+      <c r="H140" s="52">
+        <v>5.5176291592351498E-6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B141" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C141" s="56">
+        <v>-67.294371704427306</v>
+      </c>
+      <c r="D141" s="56">
+        <v>34.100185727058303</v>
+      </c>
+      <c r="E141" s="51">
+        <v>4030</v>
+      </c>
+      <c r="F141" s="51">
+        <v>-163.06749754319799</v>
+      </c>
+      <c r="G141" s="51">
+        <v>28.478754134343699</v>
+      </c>
+      <c r="H141" s="51">
+        <v>0.19821917733491001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B142" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C142" s="56">
+        <v>-131.07351750971401</v>
+      </c>
+      <c r="D142" s="56">
+        <v>34.695239645989197</v>
+      </c>
+      <c r="E142" s="51">
+        <v>4030</v>
+      </c>
+      <c r="F142" s="51">
+        <v>-228.51790034147601</v>
+      </c>
+      <c r="G142" s="51">
+        <v>-33.6291346779525</v>
+      </c>
+      <c r="H142" s="51">
+        <v>9.2258547335033502E-4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C143" s="4">
+        <v>-63.779145805286703</v>
+      </c>
+      <c r="D143" s="4">
+        <v>41.407049675645197</v>
+      </c>
+      <c r="E143" s="3">
+        <v>4030</v>
+      </c>
+      <c r="F143" s="3">
+        <v>-180.07418920884999</v>
+      </c>
+      <c r="G143" s="3">
+        <v>52.515897598276602</v>
+      </c>
+      <c r="H143" s="3">
+        <v>0.413414621546289</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>